<commit_message>
retreat bug fixed update
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Area_Data.xlsx
+++ b/GameDesign/ExcelData/Area_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill_Temp\Nameless_Temp\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC2A75-6F0C-4FF3-B284-972CC281EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DD60E2-8176-4999-AF47-E47DC31DF219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1896" yWindow="5448" windowWidth="13752" windowHeight="7428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>long</t>
   </si>
@@ -87,6 +87,10 @@
   </si>
   <si>
     <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpawnArea</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -426,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -544,10 +548,10 @@
         <v>1004</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -564,10 +568,10 @@
         <v>1005</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
spawn rule event update
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Area_Data.xlsx
+++ b/GameDesign/ExcelData/Area_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UCSC\GPM\game 271\Project\Nameless_Temp\GameDesign\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536C8304-A44A-4145-96A5-B1B64C37BECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDDBE7B-6FB2-4229-91CB-320E35AABFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,43 +102,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[6]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[3,10,4,5]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tutorial2.0_02</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[11]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[12,13,14]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Level_01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[15]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[16]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[17]</t>
+    <t>[-1,3,10,4,5]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-1,6]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-1,7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-1,11]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-1,15]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-1,16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-1,17]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[140,12,13,14]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -657,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
@@ -697,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3">
         <v>3</v>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -728,16 +728,16 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3">
         <v>3</v>
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3">
         <v>3</v>
@@ -777,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>